<commit_message>
time wise new heuristic is better but distance, not really
</commit_message>
<xml_diff>
--- a/hueristics_and_routing/heuristitcs/result.xlsx
+++ b/hueristics_and_routing/heuristitcs/result.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -416,12 +416,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>distance</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>time</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -443,10 +443,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>90.42474692456017</v>
+        <v>642.7679219733545</v>
       </c>
       <c r="E2" t="n">
-        <v>15.6034186</v>
+        <v>20.31457473333333</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -465,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>90.42474692456017</v>
+        <v>642.7679219733545</v>
       </c>
       <c r="E3" t="n">
-        <v>15.6034186</v>
+        <v>20.31457473333333</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -484,13 +484,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>376.1103167699184</v>
+        <v>597.75498125187</v>
       </c>
       <c r="E4" t="n">
-        <v>14.13070653333332</v>
+        <v>30.57566683333334</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -506,13 +506,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>376.1103167699184</v>
+        <v>477.0098043965991</v>
       </c>
       <c r="E5" t="n">
-        <v>14.13070653333332</v>
+        <v>22.88711776666668</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -521,20 +521,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>191.9859504570195</v>
+        <v>948.1799861321342</v>
       </c>
       <c r="E6" t="n">
-        <v>36.84508823333334</v>
+        <v>18.92675466666674</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -543,20 +543,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
-        <v>713.0445000303007</v>
+        <v>128.2696691792225</v>
       </c>
       <c r="E7" t="n">
-        <v>44.56986926666667</v>
+        <v>40.58960979999995</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -565,20 +565,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>713.0445000303007</v>
+        <v>874.5798335453146</v>
       </c>
       <c r="E8" t="n">
-        <v>44.56986926666667</v>
+        <v>45.60432756666671</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -587,20 +587,20 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>434.2435174184793</v>
+        <v>898.7174345861422</v>
       </c>
       <c r="E9" t="n">
-        <v>41.15908330000002</v>
+        <v>44.63159026666665</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -609,20 +609,20 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D10" t="n">
-        <v>887.0252242517308</v>
+        <v>428.7113177718129</v>
       </c>
       <c r="E10" t="n">
-        <v>53.27065206666668</v>
+        <v>4.48313306666671</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -631,20 +631,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D11" t="n">
-        <v>410.099547830614</v>
+        <v>363.6739013949409</v>
       </c>
       <c r="E11" t="n">
-        <v>29.42476406666663</v>
+        <v>28.20906950000006</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -653,20 +653,20 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>644.3958299090154</v>
+        <v>547.7573367974255</v>
       </c>
       <c r="E12" t="n">
-        <v>25.10393740000001</v>
+        <v>17.45390368333324</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -675,20 +675,20 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>614.2855477543199</v>
+        <v>547.7573367974255</v>
       </c>
       <c r="E13" t="n">
-        <v>9.547780566666688</v>
+        <v>17.45390368333324</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -697,20 +697,20 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>578.8527881979826</v>
+        <v>721.0845278754132</v>
       </c>
       <c r="E14" t="n">
-        <v>55.74687756666674</v>
+        <v>47.74245885000005</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -719,20 +719,20 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v>820.0796780213714</v>
+        <v>731.4994873754331</v>
       </c>
       <c r="E15" t="n">
-        <v>0.02318983333327651</v>
+        <v>22.02163988333336</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -741,20 +741,20 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D16" t="n">
-        <v>820.0796780213714</v>
+        <v>841.5848877596436</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02318983333327651</v>
+        <v>27.62617048333323</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D17" t="n">
-        <v>839.89766492325</v>
+        <v>293.0564817967825</v>
       </c>
       <c r="E17" t="n">
-        <v>55.63375608333342</v>
+        <v>8.144220766666649</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -785,20 +785,20 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D18" t="n">
-        <v>579.0326123644481</v>
+        <v>848.6064657588722</v>
       </c>
       <c r="E18" t="n">
-        <v>39.17503825000006</v>
+        <v>46.60815641666659</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -811,16 +811,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>678.4862561588525</v>
+        <v>303.9292160845362</v>
       </c>
       <c r="E19" t="n">
-        <v>31.11049824999998</v>
+        <v>53.70323998333333</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -833,16 +833,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D20" t="n">
-        <v>301.2174921321566</v>
+        <v>448.2121697727125</v>
       </c>
       <c r="E20" t="n">
-        <v>5.772194000000013</v>
+        <v>11.83629648333317</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -851,20 +851,20 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D21" t="n">
-        <v>271.5445023280336</v>
+        <v>186.7221115144202</v>
       </c>
       <c r="E21" t="n">
-        <v>9.414982499999951</v>
+        <v>4.422495866666623</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -873,20 +873,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
-        <v>271.5445023280336</v>
+        <v>67.15739480615593</v>
       </c>
       <c r="E22" t="n">
-        <v>9.414982499999951</v>
+        <v>56.78359380000052</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -899,16 +899,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D23" t="n">
-        <v>256.2402061795583</v>
+        <v>67.15739480615593</v>
       </c>
       <c r="E23" t="n">
-        <v>27.6885534999999</v>
+        <v>56.78359380000052</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -917,20 +917,20 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" t="n">
-        <v>504.1897267218446</v>
+        <v>861.7921812601853</v>
       </c>
       <c r="E24" t="n">
-        <v>53.14356683333335</v>
+        <v>6.86291779999965</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -939,20 +939,20 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D25" t="n">
-        <v>782.8950235222583</v>
+        <v>57.91654975304846</v>
       </c>
       <c r="E25" t="n">
-        <v>32.22722086666636</v>
+        <v>11.67415100000017</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -961,20 +961,20 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D26" t="n">
-        <v>782.8950235222583</v>
+        <v>868.2245132206008</v>
       </c>
       <c r="E26" t="n">
-        <v>32.22722086666636</v>
+        <v>29.58016979999991</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -987,16 +987,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D27" t="n">
-        <v>299.4232490418945</v>
+        <v>481.2080727429129</v>
       </c>
       <c r="E27" t="n">
-        <v>38.49111958333344</v>
+        <v>12.16152280000006</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1009,16 +1009,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>230.6041731153382</v>
+        <v>560.4315571651096</v>
       </c>
       <c r="E28" t="n">
-        <v>34.71870196666714</v>
+        <v>36.63915679999991</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1027,20 +1027,20 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C29" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D29" t="n">
-        <v>227.4096886476036</v>
+        <v>144.2584183252184</v>
       </c>
       <c r="E29" t="n">
-        <v>1.463204533334192</v>
+        <v>23.99181600000065</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1049,20 +1049,20 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>greedy</t>
+          <t>new_heuristic</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" t="n">
-        <v>227.4096886476036</v>
+        <v>232.783588927472</v>
       </c>
       <c r="E30" t="n">
-        <v>1.463204533334192</v>
+        <v>47.3355512833341</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1075,16 +1075,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>636.5405486435629</v>
+        <v>232.783588927472</v>
       </c>
       <c r="E31" t="n">
-        <v>13.67025680000006</v>
+        <v>47.3355512833341</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1097,16 +1097,16 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D32" t="n">
-        <v>773.4333700715797</v>
+        <v>553.6321877402952</v>
       </c>
       <c r="E32" t="n">
-        <v>30.36734826666702</v>
+        <v>17.04317311666637</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1119,16 +1119,16 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C33" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D33" t="n">
-        <v>997.1036191222956</v>
+        <v>916.5275729757268</v>
       </c>
       <c r="E33" t="n">
-        <v>11.64709860000005</v>
+        <v>34.67926749999924</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1141,16 +1141,16 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C34" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D34" t="n">
-        <v>752.0712815239094</v>
+        <v>916.5275729757268</v>
       </c>
       <c r="E34" t="n">
-        <v>21.3336115499992</v>
+        <v>34.67926749999924</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1166,13 +1166,13 @@
         <v>22</v>
       </c>
       <c r="C35" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D35" t="n">
-        <v>925.5467026139377</v>
+        <v>85.1124626705423</v>
       </c>
       <c r="E35" t="n">
-        <v>57.30459316666676</v>
+        <v>48.95521896666605</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1181,20 +1181,20 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>new_heuristic</t>
+          <t>greedy</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C36" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D36" t="n">
-        <v>684.3230968407588</v>
+        <v>822.6587967458181</v>
       </c>
       <c r="E36" t="n">
-        <v>18.60240250000038</v>
+        <v>4.364584666666815</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1207,18 +1207,260 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C37" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D37" t="n">
-        <v>684.3230968407588</v>
+        <v>358.2637687600218</v>
       </c>
       <c r="E37" t="n">
-        <v>18.60240250000038</v>
+        <v>57.25282379999999</v>
       </c>
       <c r="F37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>27</v>
+      </c>
+      <c r="C38" t="n">
+        <v>33</v>
+      </c>
+      <c r="D38" t="n">
+        <v>876.2048105942085</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6.243461100000786</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>27</v>
+      </c>
+      <c r="C39" t="n">
+        <v>45</v>
+      </c>
+      <c r="D39" t="n">
+        <v>124.6155862307642</v>
+      </c>
+      <c r="E39" t="n">
+        <v>7.811352450000868</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>32</v>
+      </c>
+      <c r="C40" t="n">
+        <v>38</v>
+      </c>
+      <c r="D40" t="n">
+        <v>150.6909244614653</v>
+      </c>
+      <c r="E40" t="n">
+        <v>7.829381866668882</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>32</v>
+      </c>
+      <c r="C41" t="n">
+        <v>44</v>
+      </c>
+      <c r="D41" t="n">
+        <v>520.1484631183557</v>
+      </c>
+      <c r="E41" t="n">
+        <v>54.7035493333351</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>new_heuristic</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>37</v>
+      </c>
+      <c r="C42" t="n">
+        <v>37</v>
+      </c>
+      <c r="D42" t="n">
+        <v>642.058284324361</v>
+      </c>
+      <c r="E42" t="n">
+        <v>40.4405168000003</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>37</v>
+      </c>
+      <c r="C43" t="n">
+        <v>37</v>
+      </c>
+      <c r="D43" t="n">
+        <v>642.058284324361</v>
+      </c>
+      <c r="E43" t="n">
+        <v>40.4405168000003</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>37</v>
+      </c>
+      <c r="C44" t="n">
+        <v>43</v>
+      </c>
+      <c r="D44" t="n">
+        <v>836.0277959888335</v>
+      </c>
+      <c r="E44" t="n">
+        <v>40.34617185000207</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>37</v>
+      </c>
+      <c r="C45" t="n">
+        <v>49</v>
+      </c>
+      <c r="D45" t="n">
+        <v>524.5183579868171</v>
+      </c>
+      <c r="E45" t="n">
+        <v>37.54547608333087</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>37</v>
+      </c>
+      <c r="C46" t="n">
+        <v>55</v>
+      </c>
+      <c r="D46" t="n">
+        <v>534.6393749127164</v>
+      </c>
+      <c r="E46" t="n">
+        <v>43.43480576667298</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>new_heuristic</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>42</v>
+      </c>
+      <c r="C47" t="n">
+        <v>42</v>
+      </c>
+      <c r="D47" t="n">
+        <v>687.5053024478257</v>
+      </c>
+      <c r="E47" t="n">
+        <v>40.39948190000041</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>42</v>
+      </c>
+      <c r="C48" t="n">
+        <v>42</v>
+      </c>
+      <c r="D48" t="n">
+        <v>687.5053024478257</v>
+      </c>
+      <c r="E48" t="n">
+        <v>40.39948190000041</v>
+      </c>
+      <c r="F48" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>